<commit_message>
Revision esqueleto de guion mat 11
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion01/EsqueletoGuion_MA_11_01_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion01/EsqueletoGuion_MA_11_01_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado11\guion01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18760" windowHeight="9260" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -16,18 +21,244 @@
   </sheets>
   <calcPr calcId="140001" iterateCount="2" iterateDelta="10" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Lzambrano</author>
+  </authors>
+  <commentList>
+    <comment ref="C5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lzambrano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Este texto sobra</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C65" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lzambrano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Este destacado y el recuerda no se pueden regresar a la sección 1. Son componentes de sección 2. Agregar texto antes del destacado para vincular estas secciones en el manscrito.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D86" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lzambrano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Incluir línea de texto  ajustar guion</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B87" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lzambrano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Colocar en el manuscrito una o varias líneas de texto antes del destacado.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E91" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lzambrano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Acá que hay</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F96" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lzambrano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Debe quedar dentro de una sección 2. ¿Cuál es?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D106" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lzambrano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Incluir línea de texto en manuscrito y registrarla en el esqueleto de guion</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B108" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lzambrano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Cambiar nombre por Competencias</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A109" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lzambrano:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Esto corresponde a fin de tema</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="79">
   <si>
     <t>FICHA</t>
   </si>
@@ -261,13 +492,16 @@
   </si>
   <si>
     <t>Las propiedades de orden de los números reales</t>
+  </si>
+  <si>
+    <t>Números reales</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,8 +566,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,6 +614,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -861,7 +1114,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -943,6 +1196,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="401">
@@ -1616,7 +1872,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1630,13 +1886,13 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="104.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
@@ -1644,7 +1900,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
@@ -1652,7 +1908,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="81.75" customHeight="1">
+    <row r="3" spans="1:2" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
@@ -1660,7 +1916,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -1668,7 +1924,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1676,7 +1932,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
@@ -1703,19 +1959,19 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1735,7 +1991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -1749,7 +2005,7 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -1757,7 +2013,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -1765,7 +2021,7 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -1773,16 +2029,16 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G12" s="7"/>
     </row>
   </sheetData>
@@ -1801,16 +2057,16 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView zoomScale="235" zoomScaleNormal="235" zoomScalePageLayoutView="235" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="66.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -1821,7 +2077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
         <v>37</v>
       </c>
@@ -1832,7 +2088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>40</v>
       </c>
@@ -1843,7 +2099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
         <v>35</v>
       </c>
@@ -1854,7 +2110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>75</v>
       </c>
@@ -1865,7 +2121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
         <v>45</v>
       </c>
@@ -1876,7 +2132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>46</v>
       </c>
@@ -1887,7 +2143,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>76</v>
       </c>
@@ -1898,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>77</v>
       </c>
@@ -1909,7 +2165,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>51</v>
       </c>
@@ -1920,7 +2176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>52</v>
       </c>
@@ -1931,7 +2187,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>61</v>
       </c>
@@ -1942,7 +2198,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>65</v>
       </c>
@@ -1953,7 +2209,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>66</v>
       </c>
@@ -1964,7 +2220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
         <v>69</v>
       </c>
@@ -1975,7 +2231,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
         <v>38</v>
       </c>
@@ -1986,7 +2242,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
         <v>71</v>
       </c>
@@ -1997,7 +2253,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>72</v>
       </c>
@@ -2008,7 +2264,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
         <v>73</v>
       </c>
@@ -2019,7 +2275,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>20</v>
       </c>
@@ -2030,7 +2286,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="32" t="s">
         <v>21</v>
       </c>
@@ -2041,57 +2297,57 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
       <c r="B22" s="19"/>
       <c r="C22" s="20"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="19"/>
       <c r="C24" s="19"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
@@ -2112,23 +2368,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="92.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -2139,7 +2395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -2150,7 +2406,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17">
         <v>2</v>
       </c>
@@ -2161,7 +2417,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
         <v>3</v>
       </c>
@@ -2172,7 +2428,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="16">
         <v>4</v>
       </c>
@@ -2183,7 +2439,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
         <v>5</v>
       </c>
@@ -2194,7 +2450,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="17">
         <v>6</v>
       </c>
@@ -2205,7 +2461,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
         <v>7</v>
       </c>
@@ -2216,7 +2472,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17">
         <v>8</v>
       </c>
@@ -2227,7 +2483,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>9</v>
       </c>
@@ -2238,7 +2494,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>10</v>
       </c>
@@ -2249,7 +2505,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>11</v>
       </c>
@@ -2260,7 +2516,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>12</v>
       </c>
@@ -2271,7 +2527,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="16">
         <v>13</v>
       </c>
@@ -2282,7 +2538,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>14</v>
       </c>
@@ -2293,7 +2549,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>15</v>
       </c>
@@ -2304,7 +2560,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="16">
         <v>16</v>
       </c>
@@ -2315,7 +2571,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>17</v>
       </c>
@@ -2326,7 +2582,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>18</v>
       </c>
@@ -2337,7 +2593,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="16">
         <v>19</v>
       </c>
@@ -2348,7 +2604,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>20</v>
       </c>
@@ -2375,27 +2631,27 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B50" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="42.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.33203125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="45.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.1640625" customWidth="1"/>
-    <col min="9" max="9" width="17.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="39.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="45.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -2424,9 +2680,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>39</v>
@@ -2441,9 +2697,9 @@
       <c r="H2" s="29"/>
       <c r="I2" s="29"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>39</v>
@@ -2458,9 +2714,9 @@
       <c r="H3" s="29"/>
       <c r="I3" s="29"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>39</v>
@@ -2475,14 +2731,14 @@
       <c r="H4" s="29"/>
       <c r="I4" s="29"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="48" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="41" t="s">
@@ -2496,9 +2752,9 @@
       <c r="H5" s="29"/>
       <c r="I5" s="41"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>39</v>
@@ -2515,9 +2771,9 @@
       <c r="H6" s="29"/>
       <c r="I6" s="29"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>39</v>
@@ -2534,9 +2790,9 @@
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>39</v>
@@ -2553,9 +2809,9 @@
       <c r="H8" s="29"/>
       <c r="I8" s="29"/>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>39</v>
@@ -2576,9 +2832,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B10" s="29" t="s">
         <v>39</v>
@@ -2595,9 +2851,9 @@
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>39</v>
@@ -2616,9 +2872,9 @@
       <c r="H11" s="29"/>
       <c r="I11" s="29"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>39</v>
@@ -2637,9 +2893,9 @@
       <c r="H12" s="29"/>
       <c r="I12" s="29"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>39</v>
@@ -2658,9 +2914,9 @@
       <c r="H13" s="46"/>
       <c r="I13" s="46"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B14" s="46" t="s">
         <v>39</v>
@@ -2683,9 +2939,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B15" s="46" t="s">
         <v>39</v>
@@ -2704,9 +2960,9 @@
       <c r="H15" s="46"/>
       <c r="I15" s="46"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B16" s="46" t="s">
         <v>39</v>
@@ -2725,9 +2981,9 @@
       <c r="H16" s="46"/>
       <c r="I16" s="46"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B17" s="46" t="s">
         <v>39</v>
@@ -2746,9 +3002,9 @@
       <c r="H17" s="46"/>
       <c r="I17" s="46"/>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B18" s="46" t="s">
         <v>39</v>
@@ -2767,9 +3023,9 @@
       <c r="H18" s="29"/>
       <c r="I18" s="46"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B19" s="46" t="s">
         <v>39</v>
@@ -2792,9 +3048,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B20" s="46" t="s">
         <v>39</v>
@@ -2817,9 +3073,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B21" s="46" t="s">
         <v>39</v>
@@ -2836,9 +3092,9 @@
       <c r="H21" s="29"/>
       <c r="I21" s="46"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B22" s="46" t="s">
         <v>39</v>
@@ -2855,9 +3111,9 @@
       <c r="H22" s="29"/>
       <c r="I22" s="46"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B23" s="46" t="s">
         <v>39</v>
@@ -2874,9 +3130,9 @@
       <c r="H23" s="29"/>
       <c r="I23" s="46"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B24" s="46" t="s">
         <v>39</v>
@@ -2893,9 +3149,9 @@
       <c r="H24" s="29"/>
       <c r="I24" s="46"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B25" s="46" t="s">
         <v>39</v>
@@ -2912,9 +3168,9 @@
       <c r="H25" s="46"/>
       <c r="I25" s="46"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B26" s="46" t="s">
         <v>39</v>
@@ -2931,9 +3187,9 @@
       <c r="H26" s="46"/>
       <c r="I26" s="46"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B27" s="46" t="s">
         <v>39</v>
@@ -2950,9 +3206,9 @@
       <c r="H27" s="46"/>
       <c r="I27" s="46"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B28" s="46" t="s">
         <v>39</v>
@@ -2969,9 +3225,9 @@
       <c r="H28" s="46"/>
       <c r="I28" s="46"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B29" s="46" t="s">
         <v>39</v>
@@ -2988,9 +3244,9 @@
       <c r="H29" s="46"/>
       <c r="I29" s="46"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B30" s="46" t="s">
         <v>39</v>
@@ -3007,9 +3263,9 @@
       <c r="H30" s="46"/>
       <c r="I30" s="46"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B31" s="46" t="s">
         <v>39</v>
@@ -3026,9 +3282,9 @@
       <c r="H31" s="46"/>
       <c r="I31" s="46"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B32" s="46" t="s">
         <v>39</v>
@@ -3045,9 +3301,9 @@
       <c r="H32" s="46"/>
       <c r="I32" s="46"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B33" s="46" t="s">
         <v>39</v>
@@ -3064,9 +3320,9 @@
       <c r="H33" s="46"/>
       <c r="I33" s="46"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B34" s="46" t="s">
         <v>39</v>
@@ -3083,9 +3339,9 @@
       <c r="H34" s="46"/>
       <c r="I34" s="46"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B35" s="46" t="s">
         <v>39</v>
@@ -3102,9 +3358,9 @@
       <c r="H35" s="46"/>
       <c r="I35" s="46"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B36" s="46" t="s">
         <v>39</v>
@@ -3121,9 +3377,9 @@
       <c r="H36" s="46"/>
       <c r="I36" s="46"/>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B37" s="46" t="s">
         <v>39</v>
@@ -3144,9 +3400,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B38" s="46" t="s">
         <v>39</v>
@@ -3163,9 +3419,9 @@
       <c r="H38" s="46"/>
       <c r="I38" s="46"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B39" s="46" t="s">
         <v>39</v>
@@ -3182,9 +3438,9 @@
       <c r="H39" s="46"/>
       <c r="I39" s="46"/>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B40" s="46" t="s">
         <v>39</v>
@@ -3201,9 +3457,9 @@
       <c r="H40" s="46"/>
       <c r="I40" s="46"/>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B41" s="46" t="s">
         <v>39</v>
@@ -3224,9 +3480,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B42" s="46" t="s">
         <v>39</v>
@@ -3243,9 +3499,9 @@
       <c r="H42" s="29"/>
       <c r="I42" s="46"/>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B43" s="46" t="s">
         <v>39</v>
@@ -3262,9 +3518,9 @@
       <c r="H43" s="46"/>
       <c r="I43" s="46"/>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B44" s="46" t="s">
         <v>39</v>
@@ -3285,9 +3541,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B45" s="46" t="s">
         <v>39</v>
@@ -3308,9 +3564,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B46" s="46" t="s">
         <v>39</v>
@@ -3331,9 +3587,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B47" s="46" t="s">
         <v>39</v>
@@ -3354,9 +3610,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B48" s="46" t="s">
         <v>53</v>
@@ -3371,9 +3627,9 @@
       <c r="H48" s="44"/>
       <c r="I48" s="46"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B49" s="46" t="s">
         <v>53</v>
@@ -3390,9 +3646,9 @@
       <c r="H49" s="46"/>
       <c r="I49" s="46"/>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B50" s="46" t="s">
         <v>53</v>
@@ -3409,9 +3665,9 @@
       <c r="H50" s="46"/>
       <c r="I50" s="46"/>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B51" s="46" t="s">
         <v>53</v>
@@ -3428,9 +3684,9 @@
       <c r="H51" s="46"/>
       <c r="I51" s="46"/>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B52" s="46" t="s">
         <v>53</v>
@@ -3447,9 +3703,9 @@
       <c r="H52" s="46"/>
       <c r="I52" s="46"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B53" s="46" t="s">
         <v>53</v>
@@ -3466,9 +3722,9 @@
       <c r="H53" s="29"/>
       <c r="I53" s="29"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B54" s="46" t="s">
         <v>53</v>
@@ -3485,9 +3741,9 @@
       <c r="H54" s="29"/>
       <c r="I54" s="29"/>
     </row>
-    <row r="55" spans="1:9">
-      <c r="A55" s="29" t="s">
-        <v>31</v>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B55" s="29" t="s">
         <v>53</v>
@@ -3504,9 +3760,9 @@
       <c r="H55" s="29"/>
       <c r="I55" s="29"/>
     </row>
-    <row r="56" spans="1:9">
-      <c r="A56" s="29" t="s">
-        <v>31</v>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B56" s="29" t="s">
         <v>53</v>
@@ -3523,9 +3779,9 @@
       <c r="H56" s="29"/>
       <c r="I56" s="29"/>
     </row>
-    <row r="57" spans="1:9">
-      <c r="A57" s="29" t="s">
-        <v>31</v>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B57" s="29" t="s">
         <v>53</v>
@@ -3542,9 +3798,9 @@
       <c r="H57" s="29"/>
       <c r="I57" s="29"/>
     </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="29" t="s">
-        <v>31</v>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B58" s="29" t="s">
         <v>53</v>
@@ -3561,9 +3817,9 @@
       <c r="H58" s="29"/>
       <c r="I58" s="29"/>
     </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="29" t="s">
-        <v>31</v>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B59" s="29" t="s">
         <v>53</v>
@@ -3580,9 +3836,9 @@
       <c r="H59" s="29"/>
       <c r="I59" s="29"/>
     </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="29" t="s">
-        <v>31</v>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B60" s="29" t="s">
         <v>53</v>
@@ -3599,9 +3855,9 @@
       <c r="H60" s="29"/>
       <c r="I60" s="29"/>
     </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="29" t="s">
-        <v>31</v>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B61" s="29" t="s">
         <v>53</v>
@@ -3618,9 +3874,9 @@
       <c r="H61" s="29"/>
       <c r="I61" s="29"/>
     </row>
-    <row r="62" spans="1:9">
-      <c r="A62" s="29" t="s">
-        <v>31</v>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B62" s="29" t="s">
         <v>53</v>
@@ -3637,9 +3893,9 @@
       <c r="H62" s="29"/>
       <c r="I62" s="29"/>
     </row>
-    <row r="63" spans="1:9">
-      <c r="A63" s="29" t="s">
-        <v>31</v>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B63" s="29" t="s">
         <v>53</v>
@@ -3656,9 +3912,9 @@
       <c r="H63" s="29"/>
       <c r="I63" s="29"/>
     </row>
-    <row r="64" spans="1:9">
-      <c r="A64" s="29" t="s">
-        <v>31</v>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B64" s="29" t="s">
         <v>53</v>
@@ -3675,9 +3931,9 @@
       <c r="H64" s="29"/>
       <c r="I64" s="29"/>
     </row>
-    <row r="65" spans="1:9">
-      <c r="A65" s="29" t="s">
-        <v>31</v>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B65" s="29" t="s">
         <v>53</v>
@@ -3692,9 +3948,9 @@
       <c r="H65" s="29"/>
       <c r="I65" s="29"/>
     </row>
-    <row r="66" spans="1:9">
-      <c r="A66" s="29" t="s">
-        <v>31</v>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B66" s="29" t="s">
         <v>53</v>
@@ -3709,9 +3965,9 @@
       <c r="H66" s="45"/>
       <c r="I66" s="45"/>
     </row>
-    <row r="67" spans="1:9">
-      <c r="A67" s="45" t="s">
-        <v>31</v>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B67" s="45" t="s">
         <v>53</v>
@@ -3728,9 +3984,9 @@
       <c r="H67" s="29"/>
       <c r="I67" s="29"/>
     </row>
-    <row r="68" spans="1:9">
-      <c r="A68" s="29" t="s">
-        <v>31</v>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B68" s="29" t="s">
         <v>53</v>
@@ -3749,9 +4005,9 @@
       <c r="H68" s="29"/>
       <c r="I68" s="29"/>
     </row>
-    <row r="69" spans="1:9">
-      <c r="A69" s="29" t="s">
-        <v>31</v>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B69" s="29" t="s">
         <v>53</v>
@@ -3770,9 +4026,9 @@
       <c r="H69" s="29"/>
       <c r="I69" s="29"/>
     </row>
-    <row r="70" spans="1:9">
-      <c r="A70" s="29" t="s">
-        <v>31</v>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B70" s="29" t="s">
         <v>53</v>
@@ -3791,9 +4047,9 @@
       <c r="H70" s="29"/>
       <c r="I70" s="29"/>
     </row>
-    <row r="71" spans="1:9">
-      <c r="A71" s="29" t="s">
-        <v>31</v>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B71" s="29" t="s">
         <v>53</v>
@@ -3812,9 +4068,9 @@
       <c r="H71" s="29"/>
       <c r="I71" s="29"/>
     </row>
-    <row r="72" spans="1:9">
-      <c r="A72" s="29" t="s">
-        <v>31</v>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B72" s="29" t="s">
         <v>53</v>
@@ -3833,9 +4089,9 @@
       <c r="H72" s="29"/>
       <c r="I72" s="29"/>
     </row>
-    <row r="73" spans="1:9">
-      <c r="A73" s="29" t="s">
-        <v>31</v>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B73" s="29" t="s">
         <v>53</v>
@@ -3854,9 +4110,9 @@
       <c r="H73" s="29"/>
       <c r="I73" s="29"/>
     </row>
-    <row r="74" spans="1:9">
-      <c r="A74" s="29" t="s">
-        <v>31</v>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B74" s="29" t="s">
         <v>53</v>
@@ -3875,9 +4131,9 @@
       <c r="H74" s="29"/>
       <c r="I74" s="29"/>
     </row>
-    <row r="75" spans="1:9">
-      <c r="A75" s="29" t="s">
-        <v>31</v>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B75" s="29" t="s">
         <v>53</v>
@@ -3896,9 +4152,9 @@
       <c r="H75" s="29"/>
       <c r="I75" s="29"/>
     </row>
-    <row r="76" spans="1:9">
-      <c r="A76" s="29" t="s">
-        <v>31</v>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B76" s="29" t="s">
         <v>53</v>
@@ -3917,9 +4173,9 @@
       <c r="H76" s="29"/>
       <c r="I76" s="29"/>
     </row>
-    <row r="77" spans="1:9">
-      <c r="A77" s="29" t="s">
-        <v>31</v>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B77" s="29" t="s">
         <v>53</v>
@@ -3938,9 +4194,9 @@
       <c r="H77" s="29"/>
       <c r="I77" s="29"/>
     </row>
-    <row r="78" spans="1:9">
-      <c r="A78" s="29" t="s">
-        <v>31</v>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B78" s="29" t="s">
         <v>53</v>
@@ -3959,9 +4215,9 @@
       <c r="H78" s="29"/>
       <c r="I78" s="29"/>
     </row>
-    <row r="79" spans="1:9">
-      <c r="A79" s="29" t="s">
-        <v>31</v>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B79" s="29" t="s">
         <v>53</v>
@@ -3980,9 +4236,9 @@
       <c r="H79" s="46"/>
       <c r="I79" s="46"/>
     </row>
-    <row r="80" spans="1:9">
-      <c r="A80" s="29" t="s">
-        <v>31</v>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B80" s="29" t="s">
         <v>53</v>
@@ -4001,9 +4257,9 @@
       <c r="H80" s="46"/>
       <c r="I80" s="46"/>
     </row>
-    <row r="81" spans="1:9">
-      <c r="A81" s="29" t="s">
-        <v>31</v>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B81" s="29" t="s">
         <v>53</v>
@@ -4022,9 +4278,9 @@
       <c r="H81" s="46"/>
       <c r="I81" s="46"/>
     </row>
-    <row r="82" spans="1:9">
-      <c r="A82" s="29" t="s">
-        <v>31</v>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B82" s="29" t="s">
         <v>53</v>
@@ -4043,9 +4299,9 @@
       <c r="H82" s="46"/>
       <c r="I82" s="46"/>
     </row>
-    <row r="83" spans="1:9">
-      <c r="A83" s="29" t="s">
-        <v>31</v>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B83" s="29" t="s">
         <v>53</v>
@@ -4064,9 +4320,9 @@
       <c r="H83" s="46"/>
       <c r="I83" s="46"/>
     </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="29" t="s">
-        <v>31</v>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B84" s="29" t="s">
         <v>53</v>
@@ -4085,9 +4341,9 @@
       <c r="H84" s="43"/>
       <c r="I84" s="46"/>
     </row>
-    <row r="85" spans="1:9">
-      <c r="A85" s="29" t="s">
-        <v>31</v>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B85" s="29" t="s">
         <v>53</v>
@@ -4106,9 +4362,9 @@
       <c r="H85" s="46"/>
       <c r="I85" s="46"/>
     </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="29" t="s">
-        <v>31</v>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="46" t="s">
+        <v>78</v>
       </c>
       <c r="B86" s="29" t="s">
         <v>53</v>
@@ -4129,9 +4385,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:9">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B87" s="46" t="s">
         <v>62</v>
@@ -4146,9 +4402,9 @@
       <c r="H87" s="46"/>
       <c r="I87" s="46"/>
     </row>
-    <row r="88" spans="1:9">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B88" s="46" t="s">
         <v>62</v>
@@ -4163,9 +4419,9 @@
       <c r="H88" s="46"/>
       <c r="I88" s="46"/>
     </row>
-    <row r="89" spans="1:9">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B89" s="46" t="s">
         <v>62</v>
@@ -4182,9 +4438,9 @@
       <c r="H89" s="43"/>
       <c r="I89" s="46"/>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B90" s="46" t="s">
         <v>62</v>
@@ -4201,9 +4457,9 @@
       <c r="H90" s="43"/>
       <c r="I90" s="46"/>
     </row>
-    <row r="91" spans="1:9">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B91" s="46" t="s">
         <v>62</v>
@@ -4218,9 +4474,9 @@
       <c r="H91" s="46"/>
       <c r="I91" s="46"/>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B92" s="46" t="s">
         <v>62</v>
@@ -4241,9 +4497,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B93" s="46" t="s">
         <v>62</v>
@@ -4264,9 +4520,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B94" s="46" t="s">
         <v>62</v>
@@ -4283,9 +4539,9 @@
       <c r="H94" s="46"/>
       <c r="I94" s="46"/>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B95" s="46" t="s">
         <v>62</v>
@@ -4302,9 +4558,9 @@
       <c r="H95" s="46"/>
       <c r="I95" s="46"/>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B96" s="46" t="s">
         <v>62</v>
@@ -4321,9 +4577,9 @@
       <c r="H96" s="46"/>
       <c r="I96" s="46"/>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B97" s="46" t="s">
         <v>62</v>
@@ -4340,9 +4596,9 @@
       <c r="H97" s="29"/>
       <c r="I97" s="46"/>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B98" s="46" t="s">
         <v>62</v>
@@ -4359,9 +4615,9 @@
       <c r="H98" s="29"/>
       <c r="I98" s="46"/>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B99" s="46" t="s">
         <v>62</v>
@@ -4378,9 +4634,9 @@
       <c r="H99" s="29"/>
       <c r="I99" s="46"/>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B100" s="46" t="s">
         <v>62</v>
@@ -4397,9 +4653,9 @@
       <c r="H100" s="29"/>
       <c r="I100" s="46"/>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B101" s="46" t="s">
         <v>62</v>
@@ -4420,9 +4676,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B102" s="46" t="s">
         <v>62</v>
@@ -4439,9 +4695,9 @@
       <c r="H102" s="29"/>
       <c r="I102" s="46"/>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B103" s="46" t="s">
         <v>62</v>
@@ -4458,9 +4714,9 @@
       <c r="H103" s="29"/>
       <c r="I103" s="46"/>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B104" s="46" t="s">
         <v>62</v>
@@ -4477,9 +4733,9 @@
       <c r="H104" s="29"/>
       <c r="I104" s="46"/>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B105" s="46" t="s">
         <v>62</v>
@@ -4500,9 +4756,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B106" s="46" t="s">
         <v>62</v>
@@ -4523,9 +4779,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B107" s="46" t="s">
         <v>62</v>
@@ -4546,9 +4802,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B108" s="29" t="s">
         <v>74</v>
@@ -4567,9 +4823,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B109" s="29" t="s">
         <v>20</v>
@@ -4584,9 +4840,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="46" t="s">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="B110" s="32" t="s">
         <v>21</v>
@@ -4604,6 +4860,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4618,7 +4875,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Esqueleto de guión corregido
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion01/EsqueletoGuion_MA_11_01_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion01/EsqueletoGuion_MA_11_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado11\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CristhianAndres\Documents\GitHub\Matematicas\fuentes\contenidos\grado11\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -31,234 +31,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Lzambrano</author>
-  </authors>
-  <commentList>
-    <comment ref="C5" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Lzambrano:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Este texto sobra</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C65" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Lzambrano:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Este destacado y el recuerda no se pueden regresar a la sección 1. Son componentes de sección 2. Agregar texto antes del destacado para vincular estas secciones en el manscrito.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D86" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Lzambrano:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Incluir línea de texto  ajustar guion</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B87" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Lzambrano:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Colocar en el manuscrito una o varias líneas de texto antes del destacado.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E91" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Lzambrano:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Acá que hay</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F96" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Lzambrano:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Debe quedar dentro de una sección 2. ¿Cuál es?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D106" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Lzambrano:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Incluir línea de texto en manuscrito y registrarla en el esqueleto de guion</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B108" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Lzambrano:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Cambiar nombre por Competencias</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A109" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Lzambrano:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Esto corresponde a fin de tema</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="80">
   <si>
     <t>FICHA</t>
   </si>
@@ -482,9 +256,6 @@
     <t>Competencias: Pon a prueba  tu conocimiento sobre números reales</t>
   </si>
   <si>
-    <t>Ejercitación y competencias</t>
-  </si>
-  <si>
     <t>Polinomios algebraicos de números con radicales</t>
   </si>
   <si>
@@ -495,13 +266,19 @@
   </si>
   <si>
     <t>Números reales</t>
+  </si>
+  <si>
+    <t>Competencias</t>
+  </si>
+  <si>
+    <t>Fin de tema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -566,21 +343,8 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,12 +378,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1114,7 +872,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1196,9 +954,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="401">
@@ -2056,8 +1811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView zoomScale="235" zoomScaleNormal="235" zoomScalePageLayoutView="235" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="235" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2112,7 +1867,7 @@
     </row>
     <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>19</v>
@@ -2145,7 +1900,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>36</v>
@@ -2156,7 +1911,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>19</v>
@@ -2433,7 +2188,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>19</v>
@@ -2466,7 +2221,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>19</v>
@@ -2477,7 +2232,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>19</v>
@@ -2631,11 +2386,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I110"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2682,7 +2437,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>39</v>
@@ -2699,7 +2454,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>39</v>
@@ -2716,7 +2471,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>39</v>
@@ -2733,14 +2488,12 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>22</v>
-      </c>
+      <c r="C5" s="41"/>
       <c r="D5" s="41" t="s">
         <v>32</v>
       </c>
@@ -2754,7 +2507,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>39</v>
@@ -2773,7 +2526,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>39</v>
@@ -2792,7 +2545,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>39</v>
@@ -2811,7 +2564,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>39</v>
@@ -2834,7 +2587,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="29" t="s">
         <v>39</v>
@@ -2853,7 +2606,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>39</v>
@@ -2874,7 +2627,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>39</v>
@@ -2895,7 +2648,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>39</v>
@@ -2916,7 +2669,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="46" t="s">
         <v>39</v>
@@ -2941,7 +2694,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B15" s="46" t="s">
         <v>39</v>
@@ -2962,7 +2715,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16" s="46" t="s">
         <v>39</v>
@@ -2983,7 +2736,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B17" s="46" t="s">
         <v>39</v>
@@ -3004,7 +2757,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="46" t="s">
         <v>39</v>
@@ -3025,7 +2778,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B19" s="46" t="s">
         <v>39</v>
@@ -3050,7 +2803,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" s="46" t="s">
         <v>39</v>
@@ -3075,7 +2828,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B21" s="46" t="s">
         <v>39</v>
@@ -3094,7 +2847,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22" s="46" t="s">
         <v>39</v>
@@ -3113,7 +2866,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="46" t="s">
         <v>39</v>
@@ -3132,7 +2885,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" s="46" t="s">
         <v>39</v>
@@ -3151,7 +2904,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" s="46" t="s">
         <v>39</v>
@@ -3170,7 +2923,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26" s="46" t="s">
         <v>39</v>
@@ -3189,7 +2942,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B27" s="46" t="s">
         <v>39</v>
@@ -3208,7 +2961,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B28" s="46" t="s">
         <v>39</v>
@@ -3227,7 +2980,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B29" s="46" t="s">
         <v>39</v>
@@ -3246,7 +2999,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B30" s="46" t="s">
         <v>39</v>
@@ -3265,7 +3018,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" s="46" t="s">
         <v>39</v>
@@ -3284,7 +3037,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="46" t="s">
         <v>39</v>
@@ -3303,7 +3056,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B33" s="46" t="s">
         <v>39</v>
@@ -3322,7 +3075,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B34" s="46" t="s">
         <v>39</v>
@@ -3341,7 +3094,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="46" t="s">
         <v>39</v>
@@ -3360,7 +3113,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="46" t="s">
         <v>39</v>
@@ -3379,7 +3132,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B37" s="46" t="s">
         <v>39</v>
@@ -3402,7 +3155,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B38" s="46" t="s">
         <v>39</v>
@@ -3421,7 +3174,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B39" s="46" t="s">
         <v>39</v>
@@ -3440,7 +3193,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B40" s="46" t="s">
         <v>39</v>
@@ -3459,7 +3212,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B41" s="46" t="s">
         <v>39</v>
@@ -3482,7 +3235,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B42" s="46" t="s">
         <v>39</v>
@@ -3501,7 +3254,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B43" s="46" t="s">
         <v>39</v>
@@ -3520,7 +3273,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" s="46" t="s">
         <v>39</v>
@@ -3543,7 +3296,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" s="46" t="s">
         <v>39</v>
@@ -3566,7 +3319,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B46" s="46" t="s">
         <v>39</v>
@@ -3576,26 +3329,22 @@
         <v>50</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F46" s="46"/>
       <c r="G46" s="46"/>
-      <c r="H46" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="I46" s="46" t="s">
-        <v>19</v>
-      </c>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B47" s="46" t="s">
         <v>39</v>
       </c>
       <c r="C47" s="46"/>
-      <c r="D47" s="46" t="s">
+      <c r="D47" s="47" t="s">
         <v>50</v>
       </c>
       <c r="E47" s="46" t="s">
@@ -3603,8 +3352,8 @@
       </c>
       <c r="F47" s="46"/>
       <c r="G47" s="46"/>
-      <c r="H47" s="43" t="s">
-        <v>52</v>
+      <c r="H47" s="29" t="s">
+        <v>51</v>
       </c>
       <c r="I47" s="46" t="s">
         <v>19</v>
@@ -3612,43 +3361,47 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B48" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="C48" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
+        <v>39</v>
+      </c>
+      <c r="C48" s="46"/>
+      <c r="D48" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="E48" s="46" t="s">
+        <v>26</v>
+      </c>
       <c r="F48" s="46"/>
       <c r="G48" s="46"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="46"/>
+      <c r="H48" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="I48" s="46" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B49" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C49" s="46"/>
-      <c r="D49" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="E49" s="46" t="s">
-        <v>22</v>
-      </c>
+      <c r="C49" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
       <c r="F49" s="46"/>
       <c r="G49" s="46"/>
-      <c r="H49" s="46"/>
+      <c r="H49" s="44"/>
       <c r="I49" s="46"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B50" s="46" t="s">
         <v>53</v>
@@ -3658,7 +3411,7 @@
         <v>54</v>
       </c>
       <c r="E50" s="46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F50" s="46"/>
       <c r="G50" s="46"/>
@@ -3667,7 +3420,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B51" s="46" t="s">
         <v>53</v>
@@ -3677,7 +3430,7 @@
         <v>54</v>
       </c>
       <c r="E51" s="46" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F51" s="46"/>
       <c r="G51" s="46"/>
@@ -3686,7 +3439,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B52" s="46" t="s">
         <v>53</v>
@@ -3696,7 +3449,7 @@
         <v>54</v>
       </c>
       <c r="E52" s="46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F52" s="46"/>
       <c r="G52" s="46"/>
@@ -3705,26 +3458,26 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B53" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="29"/>
+      <c r="C53" s="46"/>
       <c r="D53" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="E53" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="29"/>
-      <c r="I53" s="29"/>
+      <c r="E53" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="F53" s="46"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B54" s="46" t="s">
         <v>53</v>
@@ -3734,7 +3487,7 @@
         <v>54</v>
       </c>
       <c r="E54" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F54" s="29"/>
       <c r="G54" s="29"/>
@@ -3743,17 +3496,17 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B55" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="46" t="s">
         <v>53</v>
       </c>
       <c r="C55" s="29"/>
-      <c r="D55" s="29" t="s">
-        <v>55</v>
+      <c r="D55" s="46" t="s">
+        <v>54</v>
       </c>
       <c r="E55" s="29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F55" s="29"/>
       <c r="G55" s="29"/>
@@ -3762,7 +3515,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B56" s="29" t="s">
         <v>53</v>
@@ -3772,7 +3525,7 @@
         <v>55</v>
       </c>
       <c r="E56" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F56" s="29"/>
       <c r="G56" s="29"/>
@@ -3781,17 +3534,17 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B57" s="29" t="s">
         <v>53</v>
       </c>
       <c r="C57" s="29"/>
       <c r="D57" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E57" s="29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F57" s="29"/>
       <c r="G57" s="29"/>
@@ -3800,7 +3553,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B58" s="29" t="s">
         <v>53</v>
@@ -3810,7 +3563,7 @@
         <v>56</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F58" s="29"/>
       <c r="G58" s="29"/>
@@ -3819,7 +3572,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B59" s="29" t="s">
         <v>53</v>
@@ -3829,7 +3582,7 @@
         <v>56</v>
       </c>
       <c r="E59" s="29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F59" s="29"/>
       <c r="G59" s="29"/>
@@ -3838,7 +3591,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B60" s="29" t="s">
         <v>53</v>
@@ -3848,7 +3601,7 @@
         <v>56</v>
       </c>
       <c r="E60" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F60" s="29"/>
       <c r="G60" s="29"/>
@@ -3857,7 +3610,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B61" s="29" t="s">
         <v>53</v>
@@ -3867,7 +3620,7 @@
         <v>56</v>
       </c>
       <c r="E61" s="29" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F61" s="29"/>
       <c r="G61" s="29"/>
@@ -3876,7 +3629,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B62" s="29" t="s">
         <v>53</v>
@@ -3886,7 +3639,7 @@
         <v>56</v>
       </c>
       <c r="E62" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F62" s="29"/>
       <c r="G62" s="29"/>
@@ -3895,7 +3648,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B63" s="29" t="s">
         <v>53</v>
@@ -3905,16 +3658,16 @@
         <v>56</v>
       </c>
       <c r="E63" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F63" s="41"/>
+        <v>23</v>
+      </c>
+      <c r="F63" s="29"/>
       <c r="G63" s="29"/>
       <c r="H63" s="29"/>
       <c r="I63" s="29"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B64" s="29" t="s">
         <v>53</v>
@@ -3924,7 +3677,7 @@
         <v>56</v>
       </c>
       <c r="E64" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F64" s="41"/>
       <c r="G64" s="29"/>
@@ -3933,16 +3686,18 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B65" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C65" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="D65" s="29"/>
-      <c r="E65" s="41"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E65" s="29" t="s">
+        <v>23</v>
+      </c>
       <c r="F65" s="41"/>
       <c r="G65" s="29"/>
       <c r="H65" s="29"/>
@@ -3950,87 +3705,85 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B66" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C66" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D66" s="29"/>
-      <c r="E66" s="41"/>
-      <c r="F66" s="42"/>
-      <c r="G66" s="45"/>
-      <c r="H66" s="45"/>
-      <c r="I66" s="45"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" s="41"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="29"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B67" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B67" s="29" t="s">
         <v>53</v>
       </c>
       <c r="C67" s="29"/>
       <c r="D67" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="E67" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F67" s="29"/>
+        <v>56</v>
+      </c>
+      <c r="E67" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="F67" s="41"/>
       <c r="G67" s="29"/>
       <c r="H67" s="29"/>
       <c r="I67" s="29"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B68" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C68" s="29"/>
+      <c r="C68" s="45"/>
       <c r="D68" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="E68" s="29"/>
-      <c r="F68" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="G68" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="H68" s="29"/>
-      <c r="I68" s="29"/>
+        <v>56</v>
+      </c>
+      <c r="E68" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="F68" s="42"/>
+      <c r="G68" s="45"/>
+      <c r="H68" s="45"/>
+      <c r="I68" s="45"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B69" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69" s="45" t="s">
         <v>53</v>
       </c>
       <c r="C69" s="29"/>
       <c r="D69" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="E69" s="29"/>
-      <c r="F69" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="G69" s="29" t="s">
-        <v>22</v>
-      </c>
+      <c r="E69" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F69" s="29"/>
+      <c r="G69" s="29"/>
       <c r="H69" s="29"/>
       <c r="I69" s="29"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B70" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" s="45" t="s">
         <v>53</v>
       </c>
       <c r="C70" s="29"/>
@@ -4041,15 +3794,15 @@
       <c r="F70" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="G70" s="41" t="s">
-        <v>23</v>
+      <c r="G70" s="29" t="s">
+        <v>22</v>
       </c>
       <c r="H70" s="29"/>
       <c r="I70" s="29"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B71" s="29" t="s">
         <v>53</v>
@@ -4063,14 +3816,14 @@
         <v>58</v>
       </c>
       <c r="G71" s="29" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H71" s="29"/>
       <c r="I71" s="29"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="29" t="s">
         <v>53</v>
@@ -4083,15 +3836,15 @@
       <c r="F72" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="G72" s="41" t="s">
-        <v>23</v>
+      <c r="G72" s="29" t="s">
+        <v>22</v>
       </c>
       <c r="H72" s="29"/>
       <c r="I72" s="29"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B73" s="29" t="s">
         <v>53</v>
@@ -4104,15 +3857,15 @@
       <c r="F73" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="G73" s="29" t="s">
-        <v>22</v>
+      <c r="G73" s="41" t="s">
+        <v>23</v>
       </c>
       <c r="H73" s="29"/>
       <c r="I73" s="29"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B74" s="29" t="s">
         <v>53</v>
@@ -4123,17 +3876,17 @@
       </c>
       <c r="E74" s="29"/>
       <c r="F74" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G74" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H74" s="29"/>
       <c r="I74" s="29"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75" s="29" t="s">
         <v>53</v>
@@ -4144,17 +3897,17 @@
       </c>
       <c r="E75" s="29"/>
       <c r="F75" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="G75" s="29" t="s">
-        <v>22</v>
+        <v>58</v>
+      </c>
+      <c r="G75" s="41" t="s">
+        <v>23</v>
       </c>
       <c r="H75" s="29"/>
       <c r="I75" s="29"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B76" s="29" t="s">
         <v>53</v>
@@ -4165,17 +3918,17 @@
       </c>
       <c r="E76" s="29"/>
       <c r="F76" s="29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G76" s="29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H76" s="29"/>
       <c r="I76" s="29"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77" s="29" t="s">
         <v>53</v>
@@ -4196,7 +3949,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" s="29" t="s">
         <v>53</v>
@@ -4210,14 +3963,14 @@
         <v>59</v>
       </c>
       <c r="G78" s="29" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H78" s="29"/>
       <c r="I78" s="29"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" s="29" t="s">
         <v>53</v>
@@ -4233,12 +3986,12 @@
       <c r="G79" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H79" s="46"/>
-      <c r="I79" s="46"/>
+      <c r="H79" s="29"/>
+      <c r="I79" s="29"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" s="29" t="s">
         <v>53</v>
@@ -4249,17 +4002,17 @@
       </c>
       <c r="E80" s="29"/>
       <c r="F80" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G80" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="H80" s="46"/>
-      <c r="I80" s="46"/>
+        <v>23</v>
+      </c>
+      <c r="H80" s="29"/>
+      <c r="I80" s="29"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B81" s="29" t="s">
         <v>53</v>
@@ -4270,17 +4023,17 @@
       </c>
       <c r="E81" s="29"/>
       <c r="F81" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G81" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="H81" s="46"/>
-      <c r="I81" s="46"/>
+      <c r="H81" s="29"/>
+      <c r="I81" s="29"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B82" s="29" t="s">
         <v>53</v>
@@ -4291,17 +4044,17 @@
       </c>
       <c r="E82" s="29"/>
       <c r="F82" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G82" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="H82" s="46"/>
-      <c r="I82" s="46"/>
+      <c r="H82" s="29"/>
+      <c r="I82" s="29"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B83" s="29" t="s">
         <v>53</v>
@@ -4312,7 +4065,7 @@
       </c>
       <c r="E83" s="29"/>
       <c r="F83" s="29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G83" s="29" t="s">
         <v>22</v>
@@ -4322,7 +4075,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B84" s="29" t="s">
         <v>53</v>
@@ -4336,139 +4089,151 @@
         <v>60</v>
       </c>
       <c r="G84" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H84" s="43"/>
+        <v>22</v>
+      </c>
+      <c r="H84" s="46"/>
       <c r="I84" s="46"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B85" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C85" s="46"/>
+      <c r="C85" s="29"/>
       <c r="D85" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="E85" s="46"/>
-      <c r="F85" s="46" t="s">
+      <c r="E85" s="29"/>
+      <c r="F85" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="G85" s="46" t="s">
-        <v>22</v>
+      <c r="G85" s="29" t="s">
+        <v>25</v>
       </c>
       <c r="H85" s="46"/>
       <c r="I85" s="46"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B86" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C86" s="46"/>
-      <c r="D86" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="E86" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="F86" s="46"/>
-      <c r="G86" s="46"/>
-      <c r="H86" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="I86" s="46" t="s">
-        <v>19</v>
-      </c>
+      <c r="C86" s="29"/>
+      <c r="D86" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E86" s="29"/>
+      <c r="F86" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="G86" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H86" s="46"/>
+      <c r="I86" s="46"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B87" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="C87" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="D87" s="47"/>
-      <c r="E87" s="46"/>
-      <c r="F87" s="46"/>
-      <c r="G87" s="46"/>
+        <v>77</v>
+      </c>
+      <c r="B87" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C87" s="29"/>
+      <c r="D87" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="G87" s="29" t="s">
+        <v>23</v>
+      </c>
       <c r="H87" s="46"/>
       <c r="I87" s="46"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B88" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="C88" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="D88" s="46"/>
-      <c r="E88" s="46"/>
-      <c r="F88" s="46"/>
-      <c r="G88" s="46"/>
+        <v>77</v>
+      </c>
+      <c r="B88" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C88" s="29"/>
+      <c r="D88" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="G88" s="29" t="s">
+        <v>22</v>
+      </c>
       <c r="H88" s="46"/>
       <c r="I88" s="46"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B89" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="C89" s="46"/>
-      <c r="D89" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="E89" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="F89" s="46"/>
-      <c r="G89" s="46"/>
+        <v>77</v>
+      </c>
+      <c r="B89" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C89" s="29"/>
+      <c r="D89" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E89" s="29"/>
+      <c r="F89" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="G89" s="29" t="s">
+        <v>23</v>
+      </c>
       <c r="H89" s="43"/>
       <c r="I89" s="46"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B90" s="46" t="s">
-        <v>62</v>
+        <v>77</v>
+      </c>
+      <c r="B90" s="29" t="s">
+        <v>53</v>
       </c>
       <c r="C90" s="46"/>
-      <c r="D90" s="46" t="s">
-        <v>63</v>
-      </c>
-      <c r="E90" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="F90" s="46"/>
-      <c r="G90" s="46"/>
-      <c r="H90" s="43"/>
+      <c r="D90" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E90" s="46"/>
+      <c r="F90" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="G90" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H90" s="46"/>
       <c r="I90" s="46"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B91" s="46" t="s">
-        <v>62</v>
+        <v>77</v>
+      </c>
+      <c r="B91" s="29" t="s">
+        <v>53</v>
       </c>
       <c r="C91" s="46"/>
-      <c r="D91" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="E91" s="46"/>
+      <c r="D91" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E91" s="46" t="s">
+        <v>22</v>
+      </c>
       <c r="F91" s="46"/>
       <c r="G91" s="46"/>
       <c r="H91" s="46"/>
@@ -4476,22 +4241,22 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B92" s="46" t="s">
-        <v>62</v>
+        <v>77</v>
+      </c>
+      <c r="B92" s="29" t="s">
+        <v>53</v>
       </c>
       <c r="C92" s="46"/>
-      <c r="D92" s="46" t="s">
-        <v>64</v>
+      <c r="D92" s="47" t="s">
+        <v>50</v>
       </c>
       <c r="E92" s="46" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F92" s="46"/>
       <c r="G92" s="46"/>
-      <c r="H92" s="43" t="s">
-        <v>65</v>
+      <c r="H92" s="46" t="s">
+        <v>61</v>
       </c>
       <c r="I92" s="46" t="s">
         <v>19</v>
@@ -4499,368 +4264,543 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B93" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="C93" s="46"/>
-      <c r="D93" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="E93" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="F93" s="44"/>
+      <c r="C93" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D93" s="47"/>
+      <c r="E93" s="46"/>
+      <c r="F93" s="46"/>
       <c r="G93" s="46"/>
-      <c r="H93" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="I93" s="46" t="s">
-        <v>19</v>
-      </c>
+      <c r="H93" s="46"/>
+      <c r="I93" s="46"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B94" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="C94" s="46"/>
-      <c r="D94" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="E94" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="F94" s="44"/>
+      <c r="C94" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="D94" s="47"/>
+      <c r="E94" s="46"/>
+      <c r="F94" s="46"/>
       <c r="G94" s="46"/>
       <c r="H94" s="46"/>
       <c r="I94" s="46"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B95" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="C95" s="46"/>
-      <c r="D95" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="E95" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="F95" s="44"/>
+      <c r="C95" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D95" s="46"/>
+      <c r="E95" s="46"/>
+      <c r="F95" s="46"/>
       <c r="G95" s="46"/>
       <c r="H95" s="46"/>
       <c r="I95" s="46"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B96" s="46" t="s">
         <v>62</v>
       </c>
       <c r="C96" s="46"/>
-      <c r="D96" s="46"/>
-      <c r="E96" s="46"/>
-      <c r="F96" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="G96" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="H96" s="46"/>
+      <c r="D96" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E96" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F96" s="46"/>
+      <c r="G96" s="46"/>
+      <c r="H96" s="43"/>
       <c r="I96" s="46"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B97" s="46" t="s">
         <v>62</v>
       </c>
       <c r="C97" s="46"/>
-      <c r="D97" s="46"/>
-      <c r="E97" s="46"/>
-      <c r="F97" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="G97" s="46" t="s">
+      <c r="D97" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E97" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="H97" s="29"/>
+      <c r="F97" s="46"/>
+      <c r="G97" s="46"/>
+      <c r="H97" s="43"/>
       <c r="I97" s="46"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B98" s="46" t="s">
         <v>62</v>
       </c>
       <c r="C98" s="46"/>
-      <c r="D98" s="47"/>
-      <c r="E98" s="46"/>
-      <c r="F98" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="G98" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="H98" s="29"/>
+      <c r="D98" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E98" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F98" s="46"/>
+      <c r="G98" s="46"/>
+      <c r="H98" s="46"/>
       <c r="I98" s="46"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B99" s="46" t="s">
         <v>62</v>
       </c>
       <c r="C99" s="46"/>
-      <c r="D99" s="47"/>
-      <c r="E99" s="46"/>
-      <c r="F99" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="G99" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="H99" s="29"/>
-      <c r="I99" s="46"/>
+      <c r="D99" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E99" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="F99" s="46"/>
+      <c r="G99" s="46"/>
+      <c r="H99" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="I99" s="46" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B100" s="46" t="s">
         <v>62</v>
       </c>
       <c r="C100" s="46"/>
-      <c r="D100" s="47"/>
-      <c r="E100" s="46"/>
-      <c r="F100" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="G100" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="H100" s="29"/>
-      <c r="I100" s="46"/>
+      <c r="D100" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E100" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="F100" s="44"/>
+      <c r="G100" s="46"/>
+      <c r="H100" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="I100" s="46" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B101" s="46" t="s">
         <v>62</v>
       </c>
       <c r="C101" s="46"/>
-      <c r="D101" s="47"/>
-      <c r="E101" s="46"/>
-      <c r="F101" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="G101" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="H101" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="I101" s="46" t="s">
-        <v>19</v>
-      </c>
+      <c r="D101" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="E101" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F101" s="44"/>
+      <c r="G101" s="46"/>
+      <c r="H101" s="46"/>
+      <c r="I101" s="46"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B102" s="46" t="s">
         <v>62</v>
       </c>
       <c r="C102" s="46"/>
-      <c r="D102" s="47"/>
-      <c r="E102" s="46"/>
-      <c r="F102" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="G102" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="H102" s="29"/>
+      <c r="D102" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E102" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="F102" s="44"/>
+      <c r="G102" s="46"/>
+      <c r="H102" s="46"/>
       <c r="I102" s="46"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B103" s="46" t="s">
         <v>62</v>
       </c>
       <c r="C103" s="46"/>
-      <c r="D103" s="47"/>
+      <c r="D103" s="46" t="s">
+        <v>67</v>
+      </c>
       <c r="E103" s="46"/>
-      <c r="F103" s="46" t="s">
-        <v>70</v>
+      <c r="F103" s="44" t="s">
+        <v>68</v>
       </c>
       <c r="G103" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="H103" s="29"/>
+        <v>22</v>
+      </c>
+      <c r="H103" s="46"/>
       <c r="I103" s="46"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B104" s="46" t="s">
         <v>62</v>
       </c>
       <c r="C104" s="46"/>
-      <c r="D104" s="47"/>
+      <c r="D104" s="46" t="s">
+        <v>67</v>
+      </c>
       <c r="E104" s="46"/>
-      <c r="F104" s="46" t="s">
-        <v>70</v>
+      <c r="F104" s="44" t="s">
+        <v>68</v>
       </c>
       <c r="G104" s="46" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H104" s="29"/>
       <c r="I104" s="46"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B105" s="46" t="s">
         <v>62</v>
       </c>
       <c r="C105" s="46"/>
-      <c r="D105" s="47"/>
+      <c r="D105" s="46" t="s">
+        <v>67</v>
+      </c>
       <c r="E105" s="46"/>
-      <c r="F105" s="46" t="s">
-        <v>70</v>
+      <c r="F105" s="44" t="s">
+        <v>68</v>
       </c>
       <c r="G105" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="H105" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="I105" s="46" t="s">
-        <v>19</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H105" s="29"/>
+      <c r="I105" s="46"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B106" s="46" t="s">
         <v>62</v>
       </c>
       <c r="C106" s="46"/>
-      <c r="D106" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="E106" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="F106" s="46"/>
-      <c r="G106" s="46"/>
-      <c r="H106" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="I106" s="46" t="s">
-        <v>19</v>
-      </c>
+      <c r="D106" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E106" s="46"/>
+      <c r="F106" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="G106" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="H106" s="29"/>
+      <c r="I106" s="46"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B107" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="C107" s="29"/>
-      <c r="D107" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="E107" s="29" t="s">
-        <v>26</v>
-      </c>
-      <c r="F107" s="29"/>
-      <c r="G107" s="29"/>
-      <c r="H107" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="I107" s="29" t="s">
-        <v>19</v>
-      </c>
+      <c r="C107" s="46"/>
+      <c r="D107" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E107" s="46"/>
+      <c r="F107" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="G107" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H107" s="29"/>
+      <c r="I107" s="46"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B108" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="C108" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B108" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C108" s="46"/>
+      <c r="D108" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E108" s="46"/>
+      <c r="F108" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="G108" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D108" s="29"/>
-      <c r="E108" s="29"/>
-      <c r="F108" s="29"/>
-      <c r="G108" s="29"/>
       <c r="H108" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="I108" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="I108" s="46" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="B109" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="C109" s="29"/>
-      <c r="D109" s="41"/>
-      <c r="E109" s="41"/>
-      <c r="F109" s="41"/>
-      <c r="G109" s="41"/>
+        <v>77</v>
+      </c>
+      <c r="B109" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C109" s="46"/>
+      <c r="D109" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E109" s="46"/>
+      <c r="F109" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="G109" s="46" t="s">
+        <v>22</v>
+      </c>
       <c r="H109" s="29"/>
-      <c r="I109" s="29" t="s">
-        <v>19</v>
-      </c>
+      <c r="I109" s="46"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B110" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C110" s="46"/>
+      <c r="D110" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E110" s="46"/>
+      <c r="F110" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="G110" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="H110" s="29"/>
+      <c r="I110" s="46"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B111" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C111" s="46"/>
+      <c r="D111" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E111" s="46"/>
+      <c r="F111" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="G111" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H111" s="29"/>
+      <c r="I111" s="46"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B112" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C112" s="46"/>
+      <c r="D112" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E112" s="46"/>
+      <c r="F112" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="G112" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="H112" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="I112" s="46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B113" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C113" s="46"/>
+      <c r="D113" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="E113" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F113" s="46"/>
+      <c r="G113" s="46"/>
+      <c r="H113" s="29"/>
+      <c r="I113" s="46"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B114" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C114" s="46"/>
+      <c r="D114" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="E114" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="F114" s="46"/>
+      <c r="G114" s="46"/>
+      <c r="H114" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="I114" s="46" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B115" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C115" s="29"/>
+      <c r="D115" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="E115" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F115" s="29"/>
+      <c r="G115" s="29"/>
+      <c r="H115" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="I115" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B116" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="B110" s="32" t="s">
+      <c r="C116" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D116" s="29"/>
+      <c r="E116" s="29"/>
+      <c r="F116" s="29"/>
+      <c r="G116" s="29"/>
+      <c r="H116" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="I116" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B117" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C117" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D117" s="41"/>
+      <c r="E117" s="41"/>
+      <c r="F117" s="41"/>
+      <c r="G117" s="41"/>
+      <c r="H117" s="29"/>
+      <c r="I117" s="29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B118" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C118" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C110" s="29"/>
-      <c r="D110" s="41"/>
-      <c r="E110" s="41"/>
-      <c r="F110" s="41"/>
-      <c r="G110" s="41"/>
-      <c r="H110" s="29"/>
-      <c r="I110" s="29" t="s">
+      <c r="D118" s="41"/>
+      <c r="E118" s="41"/>
+      <c r="F118" s="41"/>
+      <c r="G118" s="41"/>
+      <c r="H118" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="I118" s="29" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
MA1101: esqueleto de guion
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion01/EsqueletoGuion_MA_11_01_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion01/EsqueletoGuion_MA_11_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado11\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado11\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21713" windowHeight="9713" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21713" windowHeight="9713" tabRatio="729" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -214,9 +214,6 @@
     <t>Evaluación</t>
   </si>
   <si>
-    <t>M102ab</t>
-  </si>
-  <si>
     <t>si</t>
   </si>
   <si>
@@ -260,6 +257,9 @@
   </si>
   <si>
     <t>Competencias</t>
+  </si>
+  <si>
+    <t>M5a</t>
   </si>
 </sst>
 </file>
@@ -1291,7 +1291,7 @@
         <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E25" t="s">
         <v>32</v>
@@ -1311,7 +1311,7 @@
         <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E26" t="s">
         <v>32</v>
@@ -1330,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1396,7 +1396,7 @@
         <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1444,7 +1444,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -1455,7 +1455,7 @@
         <v>31</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
@@ -1466,7 +1466,7 @@
         <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -1477,7 +1477,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -1488,7 +1488,7 @@
         <v>37</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -1499,7 +1499,7 @@
         <v>38</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -1510,7 +1510,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -1521,7 +1521,7 @@
         <v>42</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -1532,7 +1532,7 @@
         <v>43</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -1543,7 +1543,7 @@
         <v>44</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
@@ -1554,7 +1554,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -1565,7 +1565,7 @@
         <v>46</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -1576,7 +1576,7 @@
         <v>47</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -1587,7 +1587,7 @@
         <v>48</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
@@ -1598,7 +1598,7 @@
         <v>49</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -1609,7 +1609,7 @@
         <v>50</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
@@ -1620,7 +1620,7 @@
         <v>51</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
@@ -1631,7 +1631,7 @@
         <v>52</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -1642,7 +1642,7 @@
         <v>31</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
@@ -1653,7 +1653,7 @@
         <v>53</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -1664,7 +1664,7 @@
         <v>54</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
@@ -1675,7 +1675,7 @@
         <v>55</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -1686,7 +1686,7 @@
         <v>56</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
@@ -1694,10 +1694,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
@@ -1705,10 +1705,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
@@ -1754,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
@@ -1807,10 +1807,10 @@
         <v>20</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
@@ -1818,10 +1818,10 @@
         <v>20</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -1829,10 +1829,10 @@
         <v>20</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -1840,10 +1840,10 @@
         <v>20</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -1851,16 +1851,16 @@
         <v>20</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>31</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
@@ -1868,10 +1868,10 @@
         <v>20</v>
       </c>
       <c r="B7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -1879,10 +1879,10 @@
         <v>20</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
@@ -1890,10 +1890,10 @@
         <v>20</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
@@ -1901,10 +1901,10 @@
         <v>20</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
@@ -1912,10 +1912,10 @@
         <v>20</v>
       </c>
       <c r="B11" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
@@ -1923,10 +1923,10 @@
         <v>20</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
@@ -1934,10 +1934,10 @@
         <v>20</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
@@ -1945,10 +1945,10 @@
         <v>20</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
@@ -1956,10 +1956,10 @@
         <v>20</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
@@ -1967,10 +1967,10 @@
         <v>20</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
@@ -1978,10 +1978,10 @@
         <v>20</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
@@ -1989,10 +1989,10 @@
         <v>20</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
@@ -2000,16 +2000,16 @@
         <v>20</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H19" s="8" t="s">
         <v>37</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
@@ -2017,10 +2017,10 @@
         <v>20</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -2028,10 +2028,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
@@ -2039,10 +2039,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
@@ -2050,10 +2050,10 @@
         <v>20</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
@@ -2061,16 +2061,16 @@
         <v>20</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>38</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
@@ -2078,10 +2078,10 @@
         <v>20</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
@@ -2089,10 +2089,10 @@
         <v>20</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
@@ -2100,10 +2100,10 @@
         <v>20</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
@@ -2111,10 +2111,10 @@
         <v>20</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
@@ -2122,10 +2122,10 @@
         <v>20</v>
       </c>
       <c r="B29" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
@@ -2133,10 +2133,10 @@
         <v>20</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
@@ -2144,10 +2144,10 @@
         <v>20</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
@@ -2155,10 +2155,10 @@
         <v>20</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
@@ -2166,10 +2166,10 @@
         <v>20</v>
       </c>
       <c r="B33" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
@@ -2177,10 +2177,10 @@
         <v>20</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
@@ -2188,10 +2188,10 @@
         <v>20</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
@@ -2199,10 +2199,10 @@
         <v>20</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
@@ -2210,16 +2210,16 @@
         <v>20</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H37" s="8" t="s">
         <v>43</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
@@ -2227,10 +2227,10 @@
         <v>20</v>
       </c>
       <c r="B38" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.45">
@@ -2238,10 +2238,10 @@
         <v>20</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.45">
@@ -2249,10 +2249,10 @@
         <v>20</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
@@ -2260,10 +2260,10 @@
         <v>20</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
@@ -2271,16 +2271,16 @@
         <v>20</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H42" s="8" t="s">
         <v>44</v>
       </c>
       <c r="I42" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
@@ -2288,10 +2288,10 @@
         <v>20</v>
       </c>
       <c r="B43" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
@@ -2299,10 +2299,10 @@
         <v>20</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
@@ -2310,10 +2310,10 @@
         <v>20</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
@@ -2321,10 +2321,10 @@
         <v>20</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
@@ -2332,10 +2332,10 @@
         <v>20</v>
       </c>
       <c r="B47" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
@@ -2343,10 +2343,10 @@
         <v>20</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.45">
@@ -2354,10 +2354,10 @@
         <v>20</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.45">
@@ -2365,10 +2365,10 @@
         <v>20</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
@@ -2376,16 +2376,16 @@
         <v>20</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>46</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
@@ -2393,10 +2393,10 @@
         <v>20</v>
       </c>
       <c r="B52" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
@@ -2404,10 +2404,10 @@
         <v>20</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
@@ -2415,10 +2415,10 @@
         <v>20</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
@@ -2426,10 +2426,10 @@
         <v>20</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
@@ -2437,16 +2437,16 @@
         <v>20</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H56" s="8" t="s">
         <v>47</v>
       </c>
       <c r="I56" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
@@ -2454,13 +2454,13 @@
         <v>20</v>
       </c>
       <c r="B57" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E57" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="D57" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
@@ -2468,13 +2468,13 @@
         <v>20</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
@@ -2482,13 +2482,13 @@
         <v>20</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D59" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
@@ -2496,13 +2496,13 @@
         <v>20</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
@@ -2510,19 +2510,19 @@
         <v>20</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H61" s="8" t="s">
         <v>48</v>
       </c>
       <c r="I61" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.45">
@@ -2530,10 +2530,10 @@
         <v>20</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.45">
@@ -2541,10 +2541,10 @@
         <v>20</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.45">
@@ -2552,10 +2552,10 @@
         <v>20</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.45">
@@ -2563,10 +2563,10 @@
         <v>20</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.45">
@@ -2574,16 +2574,16 @@
         <v>20</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H66" s="8" t="s">
         <v>49</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.45">
@@ -2591,10 +2591,10 @@
         <v>20</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.45">
@@ -2602,10 +2602,10 @@
         <v>20</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.45">
@@ -2613,10 +2613,10 @@
         <v>20</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.45">
@@ -2624,10 +2624,10 @@
         <v>20</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.45">
@@ -2635,16 +2635,16 @@
         <v>20</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H71" s="8" t="s">
         <v>50</v>
       </c>
       <c r="I71" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.45">
@@ -2652,13 +2652,13 @@
         <v>20</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D72" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.45">
@@ -2666,13 +2666,13 @@
         <v>20</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.45">
@@ -2680,13 +2680,13 @@
         <v>20</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.45">
@@ -2694,13 +2694,13 @@
         <v>20</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.45">
@@ -2708,19 +2708,19 @@
         <v>20</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H76" s="8" t="s">
         <v>51</v>
       </c>
       <c r="I76" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.45">
@@ -2728,10 +2728,10 @@
         <v>20</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.45">
@@ -2739,10 +2739,10 @@
         <v>20</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.45">
@@ -2750,10 +2750,10 @@
         <v>20</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.45">
@@ -2761,10 +2761,10 @@
         <v>20</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.45">
@@ -2772,10 +2772,10 @@
         <v>20</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.45">
@@ -2783,10 +2783,10 @@
         <v>20</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.45">
@@ -2794,10 +2794,10 @@
         <v>20</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.45">
@@ -2805,10 +2805,10 @@
         <v>20</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.45">
@@ -2816,16 +2816,16 @@
         <v>20</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H85" s="8" t="s">
         <v>31</v>
       </c>
       <c r="I85" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.45">
@@ -2833,10 +2833,10 @@
         <v>20</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.45">
@@ -2844,10 +2844,10 @@
         <v>20</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.45">
@@ -2855,10 +2855,10 @@
         <v>20</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.45">
@@ -2866,10 +2866,10 @@
         <v>20</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.45">
@@ -2877,16 +2877,16 @@
         <v>20</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H90" s="8" t="s">
         <v>53</v>
       </c>
       <c r="I90" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.45">
@@ -2894,10 +2894,10 @@
         <v>20</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.45">
@@ -2905,10 +2905,10 @@
         <v>20</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C92" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.45">
@@ -2916,10 +2916,10 @@
         <v>20</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C93" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.45">
@@ -2927,10 +2927,10 @@
         <v>20</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C94" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.45">
@@ -2938,10 +2938,10 @@
         <v>20</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.45">
@@ -2949,10 +2949,10 @@
         <v>20</v>
       </c>
       <c r="B96" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.45">
@@ -2960,10 +2960,10 @@
         <v>20</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.45">
@@ -2971,10 +2971,10 @@
         <v>20</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C98" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.45">
@@ -2982,16 +2982,16 @@
         <v>20</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C99" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H99" s="8" t="s">
         <v>55</v>
       </c>
       <c r="I99" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.45">
@@ -2999,14 +2999,14 @@
         <v>20</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C100" s="8"/>
       <c r="D100" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.45">
@@ -3014,14 +3014,14 @@
         <v>20</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C101" s="8"/>
       <c r="D101" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.45">
@@ -3029,14 +3029,14 @@
         <v>20</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C102" s="8"/>
       <c r="D102" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.45">
@@ -3044,14 +3044,14 @@
         <v>20</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E103" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.45">
@@ -3059,20 +3059,20 @@
         <v>20</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H104" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I104" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.45">
@@ -3080,16 +3080,16 @@
         <v>20</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H105" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I105" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.45">
@@ -3097,7 +3097,7 @@
         <v>20</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C106" s="9" t="s">
         <v>60</v>
@@ -3111,7 +3111,7 @@
         <v>20</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C107" s="9" t="s">
         <v>62</v>

</xml_diff>